<commit_message>
Creation of fsp admin panel (#1814)
</commit_message>
<xml_diff>
--- a/backend/hct_mis_api/apps/payment/tests/test_file/pp_payment_list_invalid.xlsx
+++ b/backend/hct_mis_api/apps/payment/tests/test_file/pp_payment_list_invalid.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="24">
   <si>
     <t>payment_id</t>
   </si>
@@ -22,25 +22,28 @@
     <t>household_size</t>
   </si>
   <si>
-    <t>admin2</t>
-  </si>
-  <si>
-    <t>collector</t>
+    <t>admin_level_2</t>
+  </si>
+  <si>
+    <t>collector_name</t>
   </si>
   <si>
     <t>payment_channel</t>
   </si>
   <si>
-    <t>fsp</t>
+    <t>fsp_name</t>
   </si>
   <si>
     <t>currency</t>
   </si>
   <si>
-    <t>entitlement</t>
-  </si>
-  <si>
-    <t>entitlement_usd</t>
+    <t>entitlement_quantity</t>
+  </si>
+  <si>
+    <t>entitlement_quantity_usd</t>
+  </si>
+  <si>
+    <t>delivered_quantity</t>
   </si>
   <si>
     <t>123123</t>
@@ -101,7 +104,7 @@
       <name val="Helvetica Neue"/>
     </font>
     <font>
-      <sz val="15"/>
+      <sz val="14"/>
       <color indexed="8"/>
       <name val="Calibri"/>
     </font>
@@ -126,7 +129,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -194,13 +197,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -219,22 +237,16 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1352,7 +1364,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1365,8 +1377,10 @@
     <col min="5" max="5" width="16" style="1" customWidth="1"/>
     <col min="6" max="6" width="17" style="1" customWidth="1"/>
     <col min="7" max="7" width="15" style="1" customWidth="1"/>
-    <col min="8" max="10" width="8.85156" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.85156" style="1" customWidth="1"/>
+    <col min="8" max="8" width="8.85156" style="1" customWidth="1"/>
+    <col min="9" max="9" width="29.5859" style="1" customWidth="1"/>
+    <col min="10" max="11" width="36.6875" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="8.85156" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.55" customHeight="1">
@@ -1397,157 +1411,78 @@
       <c r="I1" t="s" s="4">
         <v>8</v>
       </c>
-      <c r="J1" t="s" s="5">
+      <c r="J1" t="s" s="6">
         <v>9</v>
+      </c>
+      <c r="K1" t="s" s="5">
+        <v>10</v>
       </c>
     </row>
     <row r="2" ht="13.55" customHeight="1">
       <c r="A2" t="s" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s" s="2">
-        <v>11</v>
-      </c>
-      <c r="C2" s="6">
+        <v>12</v>
+      </c>
+      <c r="C2" s="7">
         <v>4</v>
       </c>
       <c r="D2" t="s" s="2">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E2" t="s" s="3">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F2" t="s" s="4">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G2" t="s" s="5">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H2" t="s" s="3">
-        <v>16</v>
-      </c>
-      <c r="I2" s="7">
+        <v>17</v>
+      </c>
+      <c r="I2" s="8">
         <v>125</v>
       </c>
-      <c r="J2" s="8">
+      <c r="J2" s="9">
         <v>3637</v>
       </c>
+      <c r="K2" s="10"/>
     </row>
     <row r="3" ht="13.55" customHeight="1">
       <c r="A3" t="s" s="2">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s" s="2">
-        <v>18</v>
-      </c>
-      <c r="C3" s="6">
+        <v>19</v>
+      </c>
+      <c r="C3" s="7">
         <v>4</v>
       </c>
       <c r="D3" t="s" s="2">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E3" t="s" s="3">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F3" t="s" s="4">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G3" t="s" s="5">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H3" t="s" s="3">
-        <v>22</v>
-      </c>
-      <c r="I3" s="7">
+        <v>23</v>
+      </c>
+      <c r="I3" s="8">
         <v>123.123</v>
       </c>
-      <c r="J3" s="8">
+      <c r="J3" s="9">
         <v>3589</v>
       </c>
-    </row>
-    <row r="4" ht="13.55" customHeight="1">
-      <c r="A4" s="9"/>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="12"/>
-    </row>
-    <row r="5" ht="13.55" customHeight="1">
-      <c r="A5" s="9"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="12"/>
-    </row>
-    <row r="6" ht="13.55" customHeight="1">
-      <c r="A6" s="9"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="12"/>
-    </row>
-    <row r="7" ht="13.55" customHeight="1">
-      <c r="A7" s="9"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="12"/>
-    </row>
-    <row r="8" ht="13.55" customHeight="1">
-      <c r="A8" s="9"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="12"/>
-    </row>
-    <row r="9" ht="13.55" customHeight="1">
-      <c r="A9" s="9"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="12"/>
-    </row>
-    <row r="10" ht="13.55" customHeight="1">
-      <c r="A10" s="9"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="12"/>
+      <c r="K3" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Remove delivered quantity from entitlement template
</commit_message>
<xml_diff>
--- a/backend/hct_mis_api/apps/payment/tests/test_file/pp_payment_list_invalid.xlsx
+++ b/backend/hct_mis_api/apps/payment/tests/test_file/pp_payment_list_invalid.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="23">
   <si>
     <t>payment_id</t>
   </si>
@@ -41,9 +41,6 @@
   </si>
   <si>
     <t>entitlement_quantity_usd</t>
-  </si>
-  <si>
-    <t>delivered_quantity</t>
   </si>
   <si>
     <t>123123</t>
@@ -104,7 +101,7 @@
       <name val="Helvetica Neue"/>
     </font>
     <font>
-      <sz val="14"/>
+      <sz val="15"/>
       <color indexed="8"/>
       <name val="Calibri"/>
     </font>
@@ -129,7 +126,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -212,13 +209,109 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -249,7 +342,34 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -1364,7 +1484,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1378,9 +1498,9 @@
     <col min="6" max="6" width="17" style="1" customWidth="1"/>
     <col min="7" max="7" width="15" style="1" customWidth="1"/>
     <col min="8" max="8" width="8.85156" style="1" customWidth="1"/>
-    <col min="9" max="9" width="29.5859" style="1" customWidth="1"/>
-    <col min="10" max="11" width="36.6875" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="8.85156" style="1" customWidth="1"/>
+    <col min="9" max="9" width="29.6719" style="1" customWidth="1"/>
+    <col min="10" max="10" width="36.6719" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.85156" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.55" customHeight="1">
@@ -1414,34 +1534,31 @@
       <c r="J1" t="s" s="6">
         <v>9</v>
       </c>
-      <c r="K1" t="s" s="5">
-        <v>10</v>
-      </c>
     </row>
     <row r="2" ht="13.55" customHeight="1">
       <c r="A2" t="s" s="2">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s" s="2">
         <v>11</v>
-      </c>
-      <c r="B2" t="s" s="2">
-        <v>12</v>
       </c>
       <c r="C2" s="7">
         <v>4</v>
       </c>
       <c r="D2" t="s" s="2">
+        <v>12</v>
+      </c>
+      <c r="E2" t="s" s="3">
         <v>13</v>
       </c>
-      <c r="E2" t="s" s="3">
+      <c r="F2" t="s" s="4">
         <v>14</v>
       </c>
-      <c r="F2" t="s" s="4">
+      <c r="G2" t="s" s="5">
         <v>15</v>
       </c>
-      <c r="G2" t="s" s="5">
+      <c r="H2" t="s" s="3">
         <v>16</v>
-      </c>
-      <c r="H2" t="s" s="3">
-        <v>17</v>
       </c>
       <c r="I2" s="8">
         <v>125</v>
@@ -1449,32 +1566,31 @@
       <c r="J2" s="9">
         <v>3637</v>
       </c>
-      <c r="K2" s="10"/>
     </row>
     <row r="3" ht="13.55" customHeight="1">
       <c r="A3" t="s" s="2">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s" s="2">
         <v>18</v>
-      </c>
-      <c r="B3" t="s" s="2">
-        <v>19</v>
       </c>
       <c r="C3" s="7">
         <v>4</v>
       </c>
       <c r="D3" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="E3" t="s" s="3">
         <v>20</v>
       </c>
-      <c r="E3" t="s" s="3">
+      <c r="F3" t="s" s="4">
+        <v>14</v>
+      </c>
+      <c r="G3" t="s" s="5">
         <v>21</v>
       </c>
-      <c r="F3" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="G3" t="s" s="5">
+      <c r="H3" t="s" s="3">
         <v>22</v>
-      </c>
-      <c r="H3" t="s" s="3">
-        <v>23</v>
       </c>
       <c r="I3" s="8">
         <v>123.123</v>
@@ -1482,7 +1598,90 @@
       <c r="J3" s="9">
         <v>3589</v>
       </c>
-      <c r="K3" s="10"/>
+    </row>
+    <row r="4" ht="13.55" customHeight="1">
+      <c r="A4" s="10"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="13"/>
+    </row>
+    <row r="5" ht="13.55" customHeight="1">
+      <c r="A5" s="14"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="16"/>
+    </row>
+    <row r="6" ht="13.55" customHeight="1">
+      <c r="A6" s="14"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="16"/>
+    </row>
+    <row r="7" ht="13.55" customHeight="1">
+      <c r="A7" s="14"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="16"/>
+    </row>
+    <row r="8" ht="13.55" customHeight="1">
+      <c r="A8" s="14"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="16"/>
+    </row>
+    <row r="9" ht="13.55" customHeight="1">
+      <c r="A9" s="14"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="16"/>
+    </row>
+    <row r="10" ht="13.55" customHeight="1">
+      <c r="A10" s="17"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
add status column to payment plan export
</commit_message>
<xml_diff>
--- a/backend/hct_mis_api/apps/payment/tests/test_file/pp_payment_list_invalid.xlsx
+++ b/backend/hct_mis_api/apps/payment/tests/test_file/pp_payment_list_invalid.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="25">
   <si>
     <t>payment_id</t>
   </si>
@@ -43,6 +43,9 @@
     <t>entitlement_quantity_usd</t>
   </si>
   <si>
+    <t>status</t>
+  </si>
+  <si>
     <t>123123</t>
   </si>
   <si>
@@ -62,6 +65,9 @@
   </si>
   <si>
     <t>SBD</t>
+  </si>
+  <si>
+    <t>Pending</t>
   </si>
   <si>
     <t>654654</t>
@@ -126,7 +132,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -253,6 +259,19 @@
       <left style="thin">
         <color indexed="10"/>
       </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
       <right/>
       <top/>
       <bottom/>
@@ -278,6 +297,17 @@
       <left style="thin">
         <color indexed="10"/>
       </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
       <right/>
       <top/>
       <bottom style="thin">
@@ -305,13 +335,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -370,6 +413,15 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -1484,7 +1536,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1499,8 +1551,8 @@
     <col min="7" max="7" width="15" style="1" customWidth="1"/>
     <col min="8" max="8" width="8.85156" style="1" customWidth="1"/>
     <col min="9" max="9" width="29.6719" style="1" customWidth="1"/>
-    <col min="10" max="10" width="36.6719" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.85156" style="1" customWidth="1"/>
+    <col min="10" max="11" width="36.6719" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="8.85156" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.55" customHeight="1">
@@ -1534,69 +1586,78 @@
       <c r="J1" t="s" s="6">
         <v>9</v>
       </c>
+      <c r="K1" t="s" s="6">
+        <v>10</v>
+      </c>
     </row>
     <row r="2" ht="13.55" customHeight="1">
       <c r="A2" t="s" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s" s="2">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C2" s="7">
         <v>4</v>
       </c>
       <c r="D2" t="s" s="2">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E2" t="s" s="3">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F2" t="s" s="4">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G2" t="s" s="5">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H2" t="s" s="3">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I2" s="8">
         <v>125</v>
       </c>
       <c r="J2" s="9">
         <v>3637</v>
+      </c>
+      <c r="K2" t="s" s="6">
+        <v>18</v>
       </c>
     </row>
     <row r="3" ht="13.55" customHeight="1">
       <c r="A3" t="s" s="2">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B3" t="s" s="2">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C3" s="7">
         <v>4</v>
       </c>
       <c r="D3" t="s" s="2">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E3" t="s" s="3">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F3" t="s" s="4">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G3" t="s" s="5">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H3" t="s" s="3">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="I3" s="8">
         <v>123.123</v>
       </c>
       <c r="J3" s="9">
         <v>3589</v>
+      </c>
+      <c r="K3" t="s" s="6">
+        <v>18</v>
       </c>
     </row>
     <row r="4" ht="13.55" customHeight="1">
@@ -1610,78 +1671,85 @@
       <c r="H4" s="11"/>
       <c r="I4" s="12"/>
       <c r="J4" s="13"/>
+      <c r="K4" s="14"/>
     </row>
     <row r="5" ht="13.55" customHeight="1">
-      <c r="A5" s="14"/>
-      <c r="B5" s="15"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="16"/>
+      <c r="A5" s="15"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="17"/>
+      <c r="K5" s="18"/>
     </row>
     <row r="6" ht="13.55" customHeight="1">
-      <c r="A6" s="14"/>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="16"/>
+      <c r="A6" s="15"/>
+      <c r="B6" s="16"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="17"/>
+      <c r="K6" s="18"/>
     </row>
     <row r="7" ht="13.55" customHeight="1">
-      <c r="A7" s="14"/>
-      <c r="B7" s="15"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="15"/>
-      <c r="I7" s="15"/>
-      <c r="J7" s="16"/>
+      <c r="A7" s="15"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="17"/>
+      <c r="K7" s="18"/>
     </row>
     <row r="8" ht="13.55" customHeight="1">
-      <c r="A8" s="14"/>
-      <c r="B8" s="15"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="16"/>
+      <c r="A8" s="15"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="17"/>
+      <c r="K8" s="18"/>
     </row>
     <row r="9" ht="13.55" customHeight="1">
-      <c r="A9" s="14"/>
-      <c r="B9" s="15"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="15"/>
-      <c r="J9" s="16"/>
+      <c r="A9" s="15"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="17"/>
+      <c r="K9" s="18"/>
     </row>
     <row r="10" ht="13.55" customHeight="1">
-      <c r="A10" s="17"/>
-      <c r="B10" s="18"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="18"/>
-      <c r="J10" s="19"/>
+      <c r="A10" s="19"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="21"/>
+      <c r="K10" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
[177488] Payment Plan File Download: add Status column (#3509)
</commit_message>
<xml_diff>
--- a/backend/hct_mis_api/apps/payment/tests/test_file/pp_payment_list_invalid.xlsx
+++ b/backend/hct_mis_api/apps/payment/tests/test_file/pp_payment_list_invalid.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="25">
   <si>
     <t>payment_id</t>
   </si>
@@ -43,6 +43,9 @@
     <t>entitlement_quantity_usd</t>
   </si>
   <si>
+    <t>status</t>
+  </si>
+  <si>
     <t>123123</t>
   </si>
   <si>
@@ -62,6 +65,9 @@
   </si>
   <si>
     <t>SBD</t>
+  </si>
+  <si>
+    <t>Pending</t>
   </si>
   <si>
     <t>654654</t>
@@ -126,7 +132,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -253,6 +259,19 @@
       <left style="thin">
         <color indexed="10"/>
       </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
       <right/>
       <top/>
       <bottom/>
@@ -278,6 +297,17 @@
       <left style="thin">
         <color indexed="10"/>
       </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
       <right/>
       <top/>
       <bottom style="thin">
@@ -305,13 +335,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -370,6 +413,15 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -1484,7 +1536,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1499,8 +1551,8 @@
     <col min="7" max="7" width="15" style="1" customWidth="1"/>
     <col min="8" max="8" width="8.85156" style="1" customWidth="1"/>
     <col min="9" max="9" width="29.6719" style="1" customWidth="1"/>
-    <col min="10" max="10" width="36.6719" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.85156" style="1" customWidth="1"/>
+    <col min="10" max="11" width="36.6719" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="8.85156" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.55" customHeight="1">
@@ -1534,69 +1586,78 @@
       <c r="J1" t="s" s="6">
         <v>9</v>
       </c>
+      <c r="K1" t="s" s="6">
+        <v>10</v>
+      </c>
     </row>
     <row r="2" ht="13.55" customHeight="1">
       <c r="A2" t="s" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s" s="2">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C2" s="7">
         <v>4</v>
       </c>
       <c r="D2" t="s" s="2">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E2" t="s" s="3">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F2" t="s" s="4">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G2" t="s" s="5">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H2" t="s" s="3">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I2" s="8">
         <v>125</v>
       </c>
       <c r="J2" s="9">
         <v>3637</v>
+      </c>
+      <c r="K2" t="s" s="6">
+        <v>18</v>
       </c>
     </row>
     <row r="3" ht="13.55" customHeight="1">
       <c r="A3" t="s" s="2">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B3" t="s" s="2">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C3" s="7">
         <v>4</v>
       </c>
       <c r="D3" t="s" s="2">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E3" t="s" s="3">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F3" t="s" s="4">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G3" t="s" s="5">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H3" t="s" s="3">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="I3" s="8">
         <v>123.123</v>
       </c>
       <c r="J3" s="9">
         <v>3589</v>
+      </c>
+      <c r="K3" t="s" s="6">
+        <v>18</v>
       </c>
     </row>
     <row r="4" ht="13.55" customHeight="1">
@@ -1610,78 +1671,85 @@
       <c r="H4" s="11"/>
       <c r="I4" s="12"/>
       <c r="J4" s="13"/>
+      <c r="K4" s="14"/>
     </row>
     <row r="5" ht="13.55" customHeight="1">
-      <c r="A5" s="14"/>
-      <c r="B5" s="15"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="16"/>
+      <c r="A5" s="15"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="17"/>
+      <c r="K5" s="18"/>
     </row>
     <row r="6" ht="13.55" customHeight="1">
-      <c r="A6" s="14"/>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="16"/>
+      <c r="A6" s="15"/>
+      <c r="B6" s="16"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="17"/>
+      <c r="K6" s="18"/>
     </row>
     <row r="7" ht="13.55" customHeight="1">
-      <c r="A7" s="14"/>
-      <c r="B7" s="15"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="15"/>
-      <c r="I7" s="15"/>
-      <c r="J7" s="16"/>
+      <c r="A7" s="15"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="17"/>
+      <c r="K7" s="18"/>
     </row>
     <row r="8" ht="13.55" customHeight="1">
-      <c r="A8" s="14"/>
-      <c r="B8" s="15"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="16"/>
+      <c r="A8" s="15"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="17"/>
+      <c r="K8" s="18"/>
     </row>
     <row r="9" ht="13.55" customHeight="1">
-      <c r="A9" s="14"/>
-      <c r="B9" s="15"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="15"/>
-      <c r="J9" s="16"/>
+      <c r="A9" s="15"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="17"/>
+      <c r="K9" s="18"/>
     </row>
     <row r="10" ht="13.55" customHeight="1">
-      <c r="A10" s="17"/>
-      <c r="B10" s="18"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="18"/>
-      <c r="J10" s="19"/>
+      <c r="A10" s="19"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="21"/>
+      <c r="K10" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
[HOTFEATURE] Export Entitlement PaymentPlan: add field village (#3880)
* export entitlement pp: add new field

* upd tests

* upd more tests
</commit_message>
<xml_diff>
--- a/backend/hct_mis_api/apps/payment/tests/test_file/pp_payment_list_invalid.xlsx
+++ b/backend/hct_mis_api/apps/payment/tests/test_file/pp_payment_list_invalid.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="26">
   <si>
     <t>payment_id</t>
   </si>
@@ -23,6 +23,9 @@
   </si>
   <si>
     <t>admin_level_2</t>
+  </si>
+  <si>
+    <t>village</t>
   </si>
   <si>
     <t>collector_name</t>
@@ -695,7 +698,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -725,7 +727,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -751,7 +752,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -777,7 +777,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -803,7 +802,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -829,7 +827,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -855,7 +852,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -881,7 +877,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -907,7 +902,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -933,7 +927,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -990,7 +983,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1016,7 +1008,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1042,7 +1033,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1068,7 +1058,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1094,7 +1083,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1120,7 +1108,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1146,7 +1133,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1172,7 +1158,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1198,7 +1183,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1224,7 +1208,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1272,7 +1255,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1302,7 +1284,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1328,7 +1309,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1354,7 +1334,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1380,7 +1359,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1406,7 +1384,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1432,7 +1409,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1458,7 +1434,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1484,7 +1459,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1510,7 +1484,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1536,7 +1509,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1545,14 +1518,14 @@
     <col min="1" max="1" width="38" style="1" customWidth="1"/>
     <col min="2" max="2" width="17" style="1" customWidth="1"/>
     <col min="3" max="3" width="16" style="1" customWidth="1"/>
-    <col min="4" max="4" width="8" style="1" customWidth="1"/>
-    <col min="5" max="5" width="16" style="1" customWidth="1"/>
-    <col min="6" max="6" width="17" style="1" customWidth="1"/>
-    <col min="7" max="7" width="15" style="1" customWidth="1"/>
-    <col min="8" max="8" width="8.85156" style="1" customWidth="1"/>
-    <col min="9" max="9" width="29.6719" style="1" customWidth="1"/>
-    <col min="10" max="11" width="36.6719" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="8.85156" style="1" customWidth="1"/>
+    <col min="4" max="5" width="23.4531" style="1" customWidth="1"/>
+    <col min="6" max="6" width="16" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17" style="1" customWidth="1"/>
+    <col min="8" max="8" width="15" style="1" customWidth="1"/>
+    <col min="9" max="9" width="8.85156" style="1" customWidth="1"/>
+    <col min="10" max="10" width="29.6719" style="1" customWidth="1"/>
+    <col min="11" max="12" width="36.6719" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.85156" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.55" customHeight="1">
@@ -1568,96 +1541,101 @@
       <c r="D1" t="s" s="2">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="3">
+      <c r="E1" t="s" s="2">
         <v>4</v>
       </c>
-      <c r="F1" t="s" s="4">
+      <c r="F1" t="s" s="3">
         <v>5</v>
       </c>
-      <c r="G1" t="s" s="5">
+      <c r="G1" t="s" s="4">
         <v>6</v>
       </c>
-      <c r="H1" t="s" s="3">
+      <c r="H1" t="s" s="5">
         <v>7</v>
       </c>
-      <c r="I1" t="s" s="4">
+      <c r="I1" t="s" s="3">
         <v>8</v>
       </c>
-      <c r="J1" t="s" s="6">
+      <c r="J1" t="s" s="4">
         <v>9</v>
       </c>
       <c r="K1" t="s" s="6">
         <v>10</v>
+      </c>
+      <c r="L1" t="s" s="6">
+        <v>11</v>
       </c>
     </row>
     <row r="2" ht="13.55" customHeight="1">
       <c r="A2" t="s" s="2">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s" s="2">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C2" s="7">
         <v>4</v>
       </c>
       <c r="D2" t="s" s="2">
-        <v>13</v>
-      </c>
-      <c r="E2" t="s" s="3">
         <v>14</v>
       </c>
-      <c r="F2" t="s" s="4">
+      <c r="E2" s="2"/>
+      <c r="F2" t="s" s="3">
         <v>15</v>
       </c>
-      <c r="G2" t="s" s="5">
+      <c r="G2" t="s" s="4">
         <v>16</v>
       </c>
-      <c r="H2" t="s" s="3">
+      <c r="H2" t="s" s="5">
         <v>17</v>
       </c>
-      <c r="I2" s="8">
+      <c r="I2" t="s" s="3">
+        <v>18</v>
+      </c>
+      <c r="J2" s="8">
         <v>125</v>
       </c>
-      <c r="J2" s="9">
+      <c r="K2" s="9">
         <v>3637</v>
       </c>
-      <c r="K2" t="s" s="6">
-        <v>18</v>
+      <c r="L2" t="s" s="6">
+        <v>19</v>
       </c>
     </row>
     <row r="3" ht="13.55" customHeight="1">
       <c r="A3" t="s" s="2">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s" s="2">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C3" s="7">
         <v>4</v>
       </c>
       <c r="D3" t="s" s="2">
-        <v>21</v>
-      </c>
-      <c r="E3" t="s" s="3">
         <v>22</v>
       </c>
-      <c r="F3" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="G3" t="s" s="5">
+      <c r="E3" s="2"/>
+      <c r="F3" t="s" s="3">
         <v>23</v>
       </c>
-      <c r="H3" t="s" s="3">
+      <c r="G3" t="s" s="4">
+        <v>16</v>
+      </c>
+      <c r="H3" t="s" s="5">
         <v>24</v>
       </c>
-      <c r="I3" s="8">
+      <c r="I3" t="s" s="3">
+        <v>25</v>
+      </c>
+      <c r="J3" s="8">
         <v>123.123</v>
       </c>
-      <c r="J3" s="9">
+      <c r="K3" s="9">
         <v>3589</v>
       </c>
-      <c r="K3" t="s" s="6">
-        <v>18</v>
+      <c r="L3" t="s" s="6">
+        <v>19</v>
       </c>
     </row>
     <row r="4" ht="13.55" customHeight="1">
@@ -1666,12 +1644,13 @@
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="12"/>
       <c r="H4" s="11"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="14"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="14"/>
     </row>
     <row r="5" ht="13.55" customHeight="1">
       <c r="A5" s="15"/>
@@ -1683,8 +1662,9 @@
       <c r="G5" s="16"/>
       <c r="H5" s="16"/>
       <c r="I5" s="16"/>
-      <c r="J5" s="17"/>
-      <c r="K5" s="18"/>
+      <c r="J5" s="16"/>
+      <c r="K5" s="17"/>
+      <c r="L5" s="18"/>
     </row>
     <row r="6" ht="13.55" customHeight="1">
       <c r="A6" s="15"/>
@@ -1696,8 +1676,9 @@
       <c r="G6" s="16"/>
       <c r="H6" s="16"/>
       <c r="I6" s="16"/>
-      <c r="J6" s="17"/>
-      <c r="K6" s="18"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="17"/>
+      <c r="L6" s="18"/>
     </row>
     <row r="7" ht="13.55" customHeight="1">
       <c r="A7" s="15"/>
@@ -1709,8 +1690,9 @@
       <c r="G7" s="16"/>
       <c r="H7" s="16"/>
       <c r="I7" s="16"/>
-      <c r="J7" s="17"/>
-      <c r="K7" s="18"/>
+      <c r="J7" s="16"/>
+      <c r="K7" s="17"/>
+      <c r="L7" s="18"/>
     </row>
     <row r="8" ht="13.55" customHeight="1">
       <c r="A8" s="15"/>
@@ -1722,8 +1704,9 @@
       <c r="G8" s="16"/>
       <c r="H8" s="16"/>
       <c r="I8" s="16"/>
-      <c r="J8" s="17"/>
-      <c r="K8" s="18"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="17"/>
+      <c r="L8" s="18"/>
     </row>
     <row r="9" ht="13.55" customHeight="1">
       <c r="A9" s="15"/>
@@ -1735,8 +1718,9 @@
       <c r="G9" s="16"/>
       <c r="H9" s="16"/>
       <c r="I9" s="16"/>
-      <c r="J9" s="17"/>
-      <c r="K9" s="18"/>
+      <c r="J9" s="16"/>
+      <c r="K9" s="17"/>
+      <c r="L9" s="18"/>
     </row>
     <row r="10" ht="13.55" customHeight="1">
       <c r="A10" s="19"/>
@@ -1748,8 +1732,9 @@
       <c r="G10" s="20"/>
       <c r="H10" s="20"/>
       <c r="I10" s="20"/>
-      <c r="J10" s="21"/>
-      <c r="K10" s="22"/>
+      <c r="J10" s="20"/>
+      <c r="K10" s="21"/>
+      <c r="L10" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
[HOTFIX] 214893 Entitlement export add national id (#4245)
* add new column national_id

* upd tests

* fix tests
</commit_message>
<xml_diff>
--- a/backend/hct_mis_api/apps/payment/tests/test_file/pp_payment_list_invalid.xlsx
+++ b/backend/hct_mis_api/apps/payment/tests/test_file/pp_payment_list_invalid.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="28">
   <si>
     <t>payment_id</t>
   </si>
@@ -49,6 +49,9 @@
     <t>status</t>
   </si>
   <si>
+    <t>national_id</t>
+  </si>
+  <si>
     <t>123123</t>
   </si>
   <si>
@@ -71,6 +74,9 @@
   </si>
   <si>
     <t>Pending</t>
+  </si>
+  <si>
+    <t>123</t>
   </si>
   <si>
     <t>654654</t>
@@ -1509,7 +1515,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:L10"/>
+  <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1518,14 +1524,14 @@
     <col min="1" max="1" width="38" style="1" customWidth="1"/>
     <col min="2" max="2" width="17" style="1" customWidth="1"/>
     <col min="3" max="3" width="16" style="1" customWidth="1"/>
-    <col min="4" max="5" width="23.4531" style="1" customWidth="1"/>
+    <col min="4" max="5" width="23.5" style="1" customWidth="1"/>
     <col min="6" max="6" width="16" style="1" customWidth="1"/>
     <col min="7" max="7" width="17" style="1" customWidth="1"/>
     <col min="8" max="8" width="15" style="1" customWidth="1"/>
     <col min="9" max="9" width="8.85156" style="1" customWidth="1"/>
     <col min="10" max="10" width="29.6719" style="1" customWidth="1"/>
-    <col min="11" max="12" width="36.6719" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.85156" style="1" customWidth="1"/>
+    <col min="11" max="13" width="36.6719" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.85156" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.55" customHeight="1">
@@ -1565,32 +1571,35 @@
       <c r="L1" t="s" s="6">
         <v>11</v>
       </c>
+      <c r="M1" t="s" s="6">
+        <v>12</v>
+      </c>
     </row>
     <row r="2" ht="13.55" customHeight="1">
       <c r="A2" t="s" s="2">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C2" s="7">
         <v>4</v>
       </c>
       <c r="D2" t="s" s="2">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" t="s" s="3">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G2" t="s" s="4">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H2" t="s" s="5">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I2" t="s" s="3">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J2" s="8">
         <v>125</v>
@@ -1599,34 +1608,37 @@
         <v>3637</v>
       </c>
       <c r="L2" t="s" s="6">
-        <v>19</v>
+        <v>20</v>
+      </c>
+      <c r="M2" t="s" s="6">
+        <v>21</v>
       </c>
     </row>
     <row r="3" ht="13.55" customHeight="1">
       <c r="A3" t="s" s="2">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B3" t="s" s="2">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C3" s="7">
         <v>4</v>
       </c>
       <c r="D3" t="s" s="2">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" t="s" s="3">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="G3" t="s" s="4">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H3" t="s" s="5">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="I3" t="s" s="3">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="J3" s="8">
         <v>123.123</v>
@@ -1635,8 +1647,9 @@
         <v>3589</v>
       </c>
       <c r="L3" t="s" s="6">
-        <v>19</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="M3" s="6"/>
     </row>
     <row r="4" ht="13.55" customHeight="1">
       <c r="A4" s="10"/>
@@ -1651,6 +1664,7 @@
       <c r="J4" s="12"/>
       <c r="K4" s="13"/>
       <c r="L4" s="14"/>
+      <c r="M4" s="14"/>
     </row>
     <row r="5" ht="13.55" customHeight="1">
       <c r="A5" s="15"/>
@@ -1665,6 +1679,7 @@
       <c r="J5" s="16"/>
       <c r="K5" s="17"/>
       <c r="L5" s="18"/>
+      <c r="M5" s="18"/>
     </row>
     <row r="6" ht="13.55" customHeight="1">
       <c r="A6" s="15"/>
@@ -1679,6 +1694,7 @@
       <c r="J6" s="16"/>
       <c r="K6" s="17"/>
       <c r="L6" s="18"/>
+      <c r="M6" s="18"/>
     </row>
     <row r="7" ht="13.55" customHeight="1">
       <c r="A7" s="15"/>
@@ -1693,6 +1709,7 @@
       <c r="J7" s="16"/>
       <c r="K7" s="17"/>
       <c r="L7" s="18"/>
+      <c r="M7" s="18"/>
     </row>
     <row r="8" ht="13.55" customHeight="1">
       <c r="A8" s="15"/>
@@ -1707,6 +1724,7 @@
       <c r="J8" s="16"/>
       <c r="K8" s="17"/>
       <c r="L8" s="18"/>
+      <c r="M8" s="18"/>
     </row>
     <row r="9" ht="13.55" customHeight="1">
       <c r="A9" s="15"/>
@@ -1721,6 +1739,7 @@
       <c r="J9" s="16"/>
       <c r="K9" s="17"/>
       <c r="L9" s="18"/>
+      <c r="M9" s="18"/>
     </row>
     <row r="10" ht="13.55" customHeight="1">
       <c r="A10" s="19"/>
@@ -1735,6 +1754,7 @@
       <c r="J10" s="20"/>
       <c r="K10" s="21"/>
       <c r="L10" s="22"/>
+      <c r="M10" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
[HOTFIX] 214893 Entitlement export add national id (#4245) (#4248)
* add new column national_id

* upd tests

* fix tests

Co-authored-by: Marek Biczysko <34810846+MarekBiczysko@users.noreply.github.com>
Co-authored-by: Jan Romaniak <jan.romaniak@tivix.com>
</commit_message>
<xml_diff>
--- a/backend/hct_mis_api/apps/payment/tests/test_file/pp_payment_list_invalid.xlsx
+++ b/backend/hct_mis_api/apps/payment/tests/test_file/pp_payment_list_invalid.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="28">
   <si>
     <t>payment_id</t>
   </si>
@@ -49,6 +49,9 @@
     <t>status</t>
   </si>
   <si>
+    <t>national_id</t>
+  </si>
+  <si>
     <t>123123</t>
   </si>
   <si>
@@ -71,6 +74,9 @@
   </si>
   <si>
     <t>Pending</t>
+  </si>
+  <si>
+    <t>123</t>
   </si>
   <si>
     <t>654654</t>
@@ -1509,7 +1515,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:L10"/>
+  <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1518,14 +1524,14 @@
     <col min="1" max="1" width="38" style="1" customWidth="1"/>
     <col min="2" max="2" width="17" style="1" customWidth="1"/>
     <col min="3" max="3" width="16" style="1" customWidth="1"/>
-    <col min="4" max="5" width="23.4531" style="1" customWidth="1"/>
+    <col min="4" max="5" width="23.5" style="1" customWidth="1"/>
     <col min="6" max="6" width="16" style="1" customWidth="1"/>
     <col min="7" max="7" width="17" style="1" customWidth="1"/>
     <col min="8" max="8" width="15" style="1" customWidth="1"/>
     <col min="9" max="9" width="8.85156" style="1" customWidth="1"/>
     <col min="10" max="10" width="29.6719" style="1" customWidth="1"/>
-    <col min="11" max="12" width="36.6719" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.85156" style="1" customWidth="1"/>
+    <col min="11" max="13" width="36.6719" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.85156" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.55" customHeight="1">
@@ -1565,32 +1571,35 @@
       <c r="L1" t="s" s="6">
         <v>11</v>
       </c>
+      <c r="M1" t="s" s="6">
+        <v>12</v>
+      </c>
     </row>
     <row r="2" ht="13.55" customHeight="1">
       <c r="A2" t="s" s="2">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C2" s="7">
         <v>4</v>
       </c>
       <c r="D2" t="s" s="2">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" t="s" s="3">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G2" t="s" s="4">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H2" t="s" s="5">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I2" t="s" s="3">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J2" s="8">
         <v>125</v>
@@ -1599,34 +1608,37 @@
         <v>3637</v>
       </c>
       <c r="L2" t="s" s="6">
-        <v>19</v>
+        <v>20</v>
+      </c>
+      <c r="M2" t="s" s="6">
+        <v>21</v>
       </c>
     </row>
     <row r="3" ht="13.55" customHeight="1">
       <c r="A3" t="s" s="2">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B3" t="s" s="2">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C3" s="7">
         <v>4</v>
       </c>
       <c r="D3" t="s" s="2">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" t="s" s="3">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="G3" t="s" s="4">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H3" t="s" s="5">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="I3" t="s" s="3">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="J3" s="8">
         <v>123.123</v>
@@ -1635,8 +1647,9 @@
         <v>3589</v>
       </c>
       <c r="L3" t="s" s="6">
-        <v>19</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="M3" s="6"/>
     </row>
     <row r="4" ht="13.55" customHeight="1">
       <c r="A4" s="10"/>
@@ -1651,6 +1664,7 @@
       <c r="J4" s="12"/>
       <c r="K4" s="13"/>
       <c r="L4" s="14"/>
+      <c r="M4" s="14"/>
     </row>
     <row r="5" ht="13.55" customHeight="1">
       <c r="A5" s="15"/>
@@ -1665,6 +1679,7 @@
       <c r="J5" s="16"/>
       <c r="K5" s="17"/>
       <c r="L5" s="18"/>
+      <c r="M5" s="18"/>
     </row>
     <row r="6" ht="13.55" customHeight="1">
       <c r="A6" s="15"/>
@@ -1679,6 +1694,7 @@
       <c r="J6" s="16"/>
       <c r="K6" s="17"/>
       <c r="L6" s="18"/>
+      <c r="M6" s="18"/>
     </row>
     <row r="7" ht="13.55" customHeight="1">
       <c r="A7" s="15"/>
@@ -1693,6 +1709,7 @@
       <c r="J7" s="16"/>
       <c r="K7" s="17"/>
       <c r="L7" s="18"/>
+      <c r="M7" s="18"/>
     </row>
     <row r="8" ht="13.55" customHeight="1">
       <c r="A8" s="15"/>
@@ -1707,6 +1724,7 @@
       <c r="J8" s="16"/>
       <c r="K8" s="17"/>
       <c r="L8" s="18"/>
+      <c r="M8" s="18"/>
     </row>
     <row r="9" ht="13.55" customHeight="1">
       <c r="A9" s="15"/>
@@ -1721,6 +1739,7 @@
       <c r="J9" s="16"/>
       <c r="K9" s="17"/>
       <c r="L9" s="18"/>
+      <c r="M9" s="18"/>
     </row>
     <row r="10" ht="13.55" customHeight="1">
       <c r="A10" s="19"/>
@@ -1735,6 +1754,7 @@
       <c r="J10" s="20"/>
       <c r="K10" s="21"/>
       <c r="L10" s="22"/>
+      <c r="M10" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>